<commit_message>
Mise à jour du planning, la doc technique et le journal de bord
J'ai rajouté des tâche dans le planning, ai commencé le plan de test, ai écris beaucoup de panse-bête dans le journal de bord
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijon Rahman\Documents\GitHub\Srijon_Rahman_TPI_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9516FB0-F69E-4254-AB2C-8B1E4F65919D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CA60DA-7577-488B-A526-842331482B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-60" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -151,6 +151,12 @@
   <si>
     <t>Créer un Github pour mon projet + un trello avec un modèle Kanban</t>
   </si>
+  <si>
+    <t>Insérer une base de données avec les différentes tables</t>
+  </si>
+  <si>
+    <t>CRUD de la table jeuvideo avec ses genres et sa platform et les pegi</t>
+  </si>
 </sst>
 </file>
 
@@ -202,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -398,12 +404,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -454,36 +469,14 @@
     <xf numFmtId="20" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
-  <dxfs count="79">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="77">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -497,6 +490,11 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFC6D9F0"/>
           <bgColor rgb="FFC6D9F0"/>
@@ -513,7 +511,18 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
       </fill>
     </dxf>
     <dxf>
@@ -583,11 +592,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -600,17 +604,14 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFC6D9F0"/>
           <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -849,19 +850,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -869,6 +857,19 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1316,8 +1317,8 @@
   </sheetPr>
   <dimension ref="A1:AA999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3070,136 +3071,136 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="cellIs" dxfId="78" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C25:J25 C24:M24">
-    <cfRule type="cellIs" dxfId="75" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C25:J25 L25:M25 C24:M24">
-    <cfRule type="cellIs" dxfId="74" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="73" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C24:M24 C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="72" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:M22 D2:M4">
-    <cfRule type="cellIs" dxfId="71" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:M22">
-    <cfRule type="cellIs" dxfId="70" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="41" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M22 C10:M11 D14:M21 C15:C21">
-    <cfRule type="cellIs" dxfId="69" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="68" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="21" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22 J22">
-    <cfRule type="cellIs" dxfId="67" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="39" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23 D25 F25 H25 J25 M25">
-    <cfRule type="cellIs" dxfId="66" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="10" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M4 C5:M22">
-    <cfRule type="cellIs" dxfId="65" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="43" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M4 I5:I21">
-    <cfRule type="cellIs" dxfId="64" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="27" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M4">
-    <cfRule type="cellIs" dxfId="63" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:F23 I25">
-    <cfRule type="cellIs" dxfId="62" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="8" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G23">
-    <cfRule type="cellIs" dxfId="61" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="11" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="60" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="40" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:K23 K25:L25 D24:M24 C2:C25 E5:E23 L5:L23 E25 G25">
-    <cfRule type="cellIs" dxfId="59" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I22">
-    <cfRule type="cellIs" dxfId="58" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="35" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:K23 K25">
-    <cfRule type="cellIs" dxfId="57" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:M23 K25">
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:M23 K25:M25">
-    <cfRule type="cellIs" dxfId="54" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="53" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="30" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24">
-    <cfRule type="cellIs" dxfId="52" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N25">
-    <cfRule type="cellIs" dxfId="51" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="19" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3210,10 +3211,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA999"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3310,10 +3311,10 @@
         <v>16</v>
       </c>
       <c r="B3" s="20">
-        <v>0.1875</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="C3" s="21">
-        <v>0.1875</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="21"/>
@@ -3327,7 +3328,7 @@
       <c r="M3" s="24"/>
       <c r="N3" s="32">
         <f>SUM(C3:M3)</f>
-        <v>0.1875</v>
+        <v>0.17361111111111113</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3376,43 +3377,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>28</v>
+    <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>38</v>
       </c>
       <c r="B6" s="20">
-        <v>8.3333333333333329E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="C6" s="21">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D6" s="25">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="26"/>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E6" s="21">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="M6" s="36"/>
       <c r="N6" s="32">
         <f>SUM(C6:M6)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="21">
-        <v>0.16666666666666666</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B7" s="20">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C7" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D7" s="25">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E7" s="21"/>
       <c r="F7" s="25"/>
       <c r="G7" s="21"/>
       <c r="H7" s="25"/>
@@ -3422,15 +3419,17 @@
       <c r="L7" s="21"/>
       <c r="M7" s="26"/>
       <c r="N7" s="32">
-        <f t="shared" ref="N7:N25" si="0">SUM(C7:M7)</f>
-        <v>0.16666666666666666</v>
+        <f>SUM(C7:M7)</f>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="20"/>
+        <v>39</v>
+      </c>
+      <c r="B8" s="20">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="C8" s="21"/>
       <c r="D8" s="25"/>
       <c r="E8" s="21"/>
@@ -3443,13 +3442,13 @@
       <c r="L8" s="21"/>
       <c r="M8" s="26"/>
       <c r="N8" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N8:N26" si="0">SUM(C8:M8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="21"/>
@@ -3469,21 +3468,21 @@
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="13"/>
+      <c r="A10" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="26"/>
       <c r="N10" s="32">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3491,7 +3490,7 @@
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="12"/>
@@ -3511,127 +3510,123 @@
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="26"/>
+      <c r="A12" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="32">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="20">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C13" s="21">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D13" s="25">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E13" s="21"/>
+      <c r="A13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="21"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="25"/>
-      <c r="I13" s="21"/>
+      <c r="I13" s="22"/>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
-      <c r="L13" s="21"/>
+      <c r="L13" s="22"/>
       <c r="M13" s="26"/>
       <c r="N13" s="32">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="B14" s="20">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C14" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D14" s="25">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="26"/>
       <c r="N14" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="11">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E15" s="14"/>
+      <c r="A15" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="12"/>
+      <c r="G15" s="15"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="14"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="14"/>
       <c r="M15" s="13"/>
       <c r="N15" s="32">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B16" s="11">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="10">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E16" s="12"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E16" s="14"/>
       <c r="F16" s="10"/>
       <c r="G16" s="12"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="12"/>
+      <c r="I16" s="14"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
-      <c r="L16" s="12"/>
+      <c r="L16" s="14"/>
       <c r="M16" s="13"/>
       <c r="N16" s="32">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="11">
         <v>6.25E-2</v>
@@ -3656,18 +3651,16 @@
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="11">
-        <v>1.7361111111111112E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="10">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="E18" s="12">
-        <v>4.5138888888888888E-2</v>
-      </c>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E18" s="12"/>
       <c r="F18" s="10"/>
       <c r="G18" s="12"/>
       <c r="H18" s="10"/>
@@ -3683,13 +3676,17 @@
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="B19" s="11">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="10">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="E19" s="12">
-        <v>5.9027777777777783E-2</v>
+        <v>4.5138888888888888E-2</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="12"/>
@@ -3701,17 +3698,21 @@
       <c r="M19" s="13"/>
       <c r="N19" s="32">
         <f t="shared" si="0"/>
-        <v>5.9027777777777783E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="B20" s="11">
+        <v>5.9027777777777783E-2</v>
+      </c>
       <c r="C20" s="14"/>
       <c r="D20" s="10"/>
-      <c r="E20" s="12"/>
+      <c r="E20" s="12">
+        <v>5.9027777777777783E-2</v>
+      </c>
       <c r="F20" s="10"/>
       <c r="G20" s="12"/>
       <c r="H20" s="10"/>
@@ -3722,12 +3723,12 @@
       <c r="M20" s="13"/>
       <c r="N20" s="32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.9027777777777783E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="14"/>
@@ -3747,19 +3748,19 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>19</v>
+      <c r="A22" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="F22" s="10"/>
       <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="H22" s="10"/>
       <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
       <c r="L22" s="12"/>
       <c r="M22" s="13"/>
       <c r="N22" s="32">
@@ -3768,8 +3769,8 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>20</v>
+      <c r="A23" s="19" t="s">
+        <v>19</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -3790,19 +3791,15 @@
     </row>
     <row r="24" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="20">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C24" s="12">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D24" s="12">
-        <v>2.0833333333333332E-2</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B24" s="11">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="12">
-        <v>2.0833333333333332E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
@@ -3813,100 +3810,128 @@
       <c r="L24" s="12"/>
       <c r="M24" s="13"/>
       <c r="N24" s="32">
-        <f>SUM(C24:M24)</f>
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="20">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="C25" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D25" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E25" s="12">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="32">
+        <f>SUM(C25:M25)</f>
+        <v>5.2083333333333329E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="17">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C25" s="33">
+      <c r="B26" s="17">
+        <v>0.17708333333333334</v>
+      </c>
+      <c r="C26" s="33">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D26" s="34">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E25" s="12">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="32">
+      <c r="E26" s="34">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="32">
         <f t="shared" si="0"/>
-        <v>0.10416666666666666</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="10">
-        <f t="shared" ref="B26:M26" si="1">SUM(B2:B25)</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C26" s="10">
-        <f t="shared" si="1"/>
+        <v>0.17708333333333331</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="10">
+        <f>SUM(B2:B26)</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="10">
+        <f>SUM(C2:C26)</f>
         <v>0.33333333333333326</v>
       </c>
-      <c r="D26" s="10">
-        <f t="shared" si="1"/>
+      <c r="D27" s="10">
+        <f>SUM(D2:D26)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E26" s="10">
-        <f t="shared" si="1"/>
+      <c r="E27" s="10">
+        <f>SUM(E2:E26)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F26" s="10">
-        <f t="shared" si="1"/>
+      <c r="F27" s="10">
+        <f>SUM(F2:F26)</f>
         <v>0</v>
       </c>
-      <c r="G26" s="10">
-        <f t="shared" si="1"/>
+      <c r="G27" s="10">
+        <f>SUM(G2:G26)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="10">
-        <f t="shared" si="1"/>
+      <c r="H27" s="10">
+        <f>SUM(H2:H26)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="10">
-        <f t="shared" si="1"/>
+      <c r="I27" s="10">
+        <f>SUM(I2:I26)</f>
         <v>0</v>
       </c>
-      <c r="J26" s="10">
-        <f t="shared" si="1"/>
+      <c r="J27" s="10">
+        <f>SUM(J2:J26)</f>
         <v>0</v>
       </c>
-      <c r="K26" s="10">
-        <f t="shared" si="1"/>
+      <c r="K27" s="10">
+        <f>SUM(K2:K26)</f>
         <v>0</v>
       </c>
-      <c r="L26" s="10">
-        <f t="shared" si="1"/>
+      <c r="L27" s="10">
+        <f>SUM(L2:L26)</f>
         <v>0</v>
       </c>
-      <c r="M26" s="10">
-        <f t="shared" si="1"/>
+      <c r="M27" s="10">
+        <f>SUM(M2:M26)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M27" s="10">
-        <f>SUM(C26:M26)</f>
+    <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="10">
+        <f>SUM(C27:M27)</f>
         <v>0.99999999999999978</v>
       </c>
-      <c r="N27" s="10">
-        <f>SUM(N2:N25)</f>
+      <c r="N28" s="10">
+        <f>SUM(N2:N26)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4878,240 +4903,227 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C4">
-    <cfRule type="cellIs" dxfId="50" priority="41" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="40" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="39" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C25">
-    <cfRule type="cellIs" dxfId="47" priority="21" operator="greaterThan">
+  <conditionalFormatting sqref="C2:C6">
+    <cfRule type="cellIs" dxfId="48" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="43" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="44" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5 I7:I22 G5 G7:G24 L5 L7:L24 C2:C26 E5:E26">
+    <cfRule type="cellIs" dxfId="45" priority="24" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
-    <cfRule type="cellIs" dxfId="46" priority="22" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="24" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
+  <conditionalFormatting sqref="C26">
     <cfRule type="cellIs" dxfId="44" priority="25" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23:D24 F25:J25 L25:M25 F24:M24 F23:H23">
-    <cfRule type="cellIs" dxfId="43" priority="38" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25:J25 C23:D24 F24:M24 F23:H23">
-    <cfRule type="cellIs" dxfId="42" priority="33" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F25:J25 L25:M25 C23:D24 F24:M24 F23:H23">
-    <cfRule type="cellIs" dxfId="41" priority="37" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23:D23 F25:J25 L25:M25 F23:H23">
+    <cfRule type="cellIs" dxfId="43" priority="27" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="28" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:D25 F26:J26 L26:M26 F25:M25 F24:H24 D5 C7:D15 E7:M23 E2:M5">
+    <cfRule type="cellIs" dxfId="41" priority="41" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:J26 C24:D25 F25:M25 F24:H24 C7:D15 E7:M23 D5:M5">
     <cfRule type="cellIs" dxfId="40" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:D22 C5:D14 C15:C18 D2:D4 F2:M22">
-    <cfRule type="cellIs" dxfId="39" priority="51" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19:D22 F19:M22">
-    <cfRule type="cellIs" dxfId="38" priority="50" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22:D22 D19:D21 C15:C21 C5:D14 F5:M22">
-    <cfRule type="cellIs" dxfId="37" priority="47" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="36" priority="55" operator="equal">
+  <conditionalFormatting sqref="F26:J26 L26:M26 C24:D25 F25:M25 F24:H24 D5 C7:D15 E7:M23 E2:M5">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:D24 F26:J26 L26:M26 F24:H24">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:D23 C16:C19 D2:D4">
+    <cfRule type="cellIs" dxfId="37" priority="54" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:D23 F20:M23">
+    <cfRule type="cellIs" dxfId="36" priority="53" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:D23 D20:D22 C16:C22">
+    <cfRule type="cellIs" dxfId="35" priority="50" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:M27">
+    <cfRule type="cellIs" dxfId="34" priority="58" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D18">
-    <cfRule type="cellIs" dxfId="35" priority="12" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="14" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
+  <conditionalFormatting sqref="D16:D19">
     <cfRule type="cellIs" dxfId="33" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22 J22">
-    <cfRule type="cellIs" dxfId="32" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="18" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23 J23">
+    <cfRule type="cellIs" dxfId="30" priority="51" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D23 F25 H25 J25 M25">
-    <cfRule type="cellIs" dxfId="31" priority="34" operator="greaterThan">
+  <conditionalFormatting sqref="D24 F26 H26 J26 M26">
+    <cfRule type="cellIs" dxfId="29" priority="37" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="18" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
+  <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="28" priority="19" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="20" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="26" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4 C5:D14 C15:C18 C19:D22 F2:M22">
-    <cfRule type="cellIs" dxfId="25" priority="52" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4 I5:I21 F2:M4">
-    <cfRule type="cellIs" dxfId="24" priority="43" operator="greaterThan">
+  <conditionalFormatting sqref="D2:D4 C16:C19 C20:D23">
+    <cfRule type="cellIs" dxfId="23" priority="55" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D4 F2:M4">
+    <cfRule type="cellIs" dxfId="22" priority="46" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D4 F2:M4">
-    <cfRule type="cellIs" dxfId="23" priority="44" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F23 I25">
-    <cfRule type="cellIs" dxfId="22" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="47" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23:F24 I26">
+    <cfRule type="cellIs" dxfId="20" priority="35" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G23">
-    <cfRule type="cellIs" dxfId="21" priority="35" operator="greaterThan">
+  <conditionalFormatting sqref="G23">
+    <cfRule type="cellIs" dxfId="19" priority="52" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="20" priority="49" operator="greaterThan">
+  <conditionalFormatting sqref="G24:K24 K26:L26 D25 G26 F25:M25">
+    <cfRule type="cellIs" dxfId="18" priority="31" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G23:K23 K25:L25 D24 L5:L23 G25 F24:M24">
-    <cfRule type="cellIs" dxfId="19" priority="28" operator="greaterThan">
+  <conditionalFormatting sqref="H23:I23">
+    <cfRule type="cellIs" dxfId="17" priority="49" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22:I22">
-    <cfRule type="cellIs" dxfId="18" priority="46" operator="greaterThan">
+  <conditionalFormatting sqref="I24:K24 K26">
+    <cfRule type="cellIs" dxfId="16" priority="30" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24:M24 K26">
+    <cfRule type="cellIs" dxfId="15" priority="33" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="34" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24:M24 K26:M26">
+    <cfRule type="cellIs" dxfId="13" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="cellIs" dxfId="12" priority="48" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I23:K23 K25">
-    <cfRule type="cellIs" dxfId="17" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23:M23 K25">
-    <cfRule type="cellIs" dxfId="16" priority="31" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="30" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I23:M23 K25:M25">
-    <cfRule type="cellIs" dxfId="14" priority="29" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="13" priority="45" operator="greaterThan">
+  <conditionalFormatting sqref="M25">
+    <cfRule type="cellIs" dxfId="11" priority="29" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N26">
+    <cfRule type="cellIs" dxfId="10" priority="45" operator="equal">
+      <formula>$B2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:E26">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:E26">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24 E26">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:E26">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E12 E15:E23">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M24">
-    <cfRule type="cellIs" dxfId="12" priority="26" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N25">
-    <cfRule type="cellIs" dxfId="11" priority="42" operator="equal">
-      <formula>$B2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E25">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E25">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23 E25">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:E25">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E22">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E22">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E11 E14:E22">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E22">
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
-      <formula>0.00001157407407</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E4">
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>0.00001157407407</formula>
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Mis à jour du code
Fini la partie de l'utilisateur + début de la partie pour les jeux vidéo
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijon Rahman\Documents\GitHub\Srijon_Rahman_TPI_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CA60DA-7577-488B-A526-842331482B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9161BF1-4A51-42B2-8F0C-DA1654960F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-60" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -155,7 +155,7 @@
     <t>Insérer une base de données avec les différentes tables</t>
   </si>
   <si>
-    <t>CRUD de la table jeuvideo avec ses genres et sa platform et les pegi</t>
+    <t>Faire les fonction entre la table jeuvideo et la table pegi, même chose pour les notes</t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -413,6 +413,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -470,13 +481,127 @@
     <xf numFmtId="20" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
-  <dxfs count="77">
+  <dxfs count="91">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1318,7 +1443,7 @@
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3071,136 +3196,136 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="cellIs" dxfId="76" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C25:J25 C24:M24">
-    <cfRule type="cellIs" dxfId="73" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C25:J25 L25:M25 C24:M24">
-    <cfRule type="cellIs" dxfId="72" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="71" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C24:M24 C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="70" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:M22 D2:M4">
-    <cfRule type="cellIs" dxfId="69" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:M22">
-    <cfRule type="cellIs" dxfId="68" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="41" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M22 C10:M11 D14:M21 C15:C21">
-    <cfRule type="cellIs" dxfId="67" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="66" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="21" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22 J22">
-    <cfRule type="cellIs" dxfId="65" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="39" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23 D25 F25 H25 J25 M25">
-    <cfRule type="cellIs" dxfId="64" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="10" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M4 C5:M22">
-    <cfRule type="cellIs" dxfId="63" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="43" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M4 I5:I21">
-    <cfRule type="cellIs" dxfId="62" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="27" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M4">
-    <cfRule type="cellIs" dxfId="61" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:F23 I25">
-    <cfRule type="cellIs" dxfId="60" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="8" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G23">
-    <cfRule type="cellIs" dxfId="59" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="11" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="58" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="40" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:K23 K25:L25 D24:M24 C2:C25 E5:E23 L5:L23 E25 G25">
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I22">
-    <cfRule type="cellIs" dxfId="56" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="35" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:K23 K25">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:M23 K25">
-    <cfRule type="cellIs" dxfId="54" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:M23 K25:M25">
-    <cfRule type="cellIs" dxfId="52" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="51" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="30" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24">
-    <cfRule type="cellIs" dxfId="50" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N25">
-    <cfRule type="cellIs" dxfId="49" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="19" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3211,15 +3336,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="60.875" customWidth="1"/>
+    <col min="1" max="1" width="62.25" customWidth="1"/>
     <col min="2" max="2" width="11.375" customWidth="1"/>
     <col min="3" max="27" width="10" customWidth="1"/>
   </cols>
@@ -3240,7 +3365,7 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="37" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -3293,7 +3418,7 @@
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="18"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
@@ -3302,7 +3427,7 @@
       <c r="L2" s="8"/>
       <c r="M2" s="9"/>
       <c r="N2" s="32">
-        <f>SUM(C2:M2)</f>
+        <f t="shared" ref="N2:N7" si="0">SUM(C2:M2)</f>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -3327,7 +3452,7 @@
       <c r="L3" s="22"/>
       <c r="M3" s="24"/>
       <c r="N3" s="32">
-        <f>SUM(C3:M3)</f>
+        <f t="shared" si="0"/>
         <v>0.17361111111111113</v>
       </c>
     </row>
@@ -3352,7 +3477,7 @@
       <c r="L4" s="22"/>
       <c r="M4" s="24"/>
       <c r="N4" s="32">
-        <f>SUM(C4:M4)</f>
+        <f t="shared" si="0"/>
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
@@ -3364,7 +3489,7 @@
       <c r="C5" s="21"/>
       <c r="D5" s="25"/>
       <c r="E5" s="21"/>
-      <c r="F5" s="25"/>
+      <c r="F5" s="22"/>
       <c r="G5" s="21"/>
       <c r="H5" s="25"/>
       <c r="I5" s="21"/>
@@ -3373,12 +3498,12 @@
       <c r="L5" s="21"/>
       <c r="M5" s="26"/>
       <c r="N5" s="32">
-        <f>SUM(C5:M5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="28" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="20">
@@ -3390,10 +3515,13 @@
       <c r="E6" s="21">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="F6" s="21">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="M6" s="36"/>
       <c r="N6" s="32">
-        <f>SUM(C6:M6)</f>
-        <v>5.5555555555555552E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.5972222222222224E-2</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3419,21 +3547,21 @@
       <c r="L7" s="21"/>
       <c r="M7" s="26"/>
       <c r="N7" s="32">
-        <f>SUM(C7:M7)</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="20">
-        <v>2.0833333333333332E-2</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B8" s="20"/>
       <c r="C8" s="21"/>
       <c r="D8" s="25"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="25"/>
+      <c r="F8" s="25">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G8" s="21"/>
       <c r="H8" s="25"/>
       <c r="I8" s="21"/>
@@ -3442,13 +3570,13 @@
       <c r="L8" s="21"/>
       <c r="M8" s="26"/>
       <c r="N8" s="32">
-        <f t="shared" ref="N8:N26" si="0">SUM(C8:M8)</f>
-        <v>0</v>
+        <f t="shared" ref="N8:N27" si="1">SUM(C8:M8)</f>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="21"/>
@@ -3462,20 +3590,19 @@
       <c r="K9" s="25"/>
       <c r="L9" s="21"/>
       <c r="M9" s="26"/>
-      <c r="N9" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="N9" s="32"/>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="21"/>
       <c r="D10" s="25"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="25"/>
+      <c r="F10" s="25">
+        <v>4.8611111111111112E-2</v>
+      </c>
       <c r="G10" s="21"/>
       <c r="H10" s="25"/>
       <c r="I10" s="21"/>
@@ -3484,34 +3611,36 @@
       <c r="L10" s="21"/>
       <c r="M10" s="26"/>
       <c r="N10" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>4.8611111111111112E-2</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="13"/>
+      <c r="A11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="25">
+        <v>5.9027777777777783E-2</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="26"/>
       <c r="N11" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5.9027777777777783E-2</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
@@ -3526,132 +3655,127 @@
       <c r="L12" s="12"/>
       <c r="M12" s="13"/>
       <c r="N12" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="20">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C14" s="21">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D14" s="25">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E14" s="21"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="25"/>
-      <c r="G14" s="21"/>
+      <c r="G14" s="22"/>
       <c r="H14" s="25"/>
-      <c r="I14" s="21"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
-      <c r="L14" s="21"/>
+      <c r="L14" s="22"/>
       <c r="M14" s="26"/>
       <c r="N14" s="32">
-        <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="20">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C15" s="21">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D15" s="25">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="32">
+        <f t="shared" si="1"/>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="11">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="10">
-        <v>5.5555555555555552E-2</v>
-      </c>
-      <c r="E16" s="14"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="15"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="14"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="14"/>
       <c r="M16" s="13"/>
       <c r="N16" s="32">
-        <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B17" s="11">
-        <v>6.25E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="10">
-        <v>6.25E-2</v>
-      </c>
-      <c r="E17" s="12"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E17" s="14"/>
       <c r="F17" s="10"/>
       <c r="G17" s="12"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="12"/>
+      <c r="I17" s="14"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
-      <c r="L17" s="12"/>
+      <c r="L17" s="14"/>
       <c r="M17" s="13"/>
       <c r="N17" s="32">
-        <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="11">
         <v>6.25E-2</v>
@@ -3670,24 +3794,22 @@
       <c r="L18" s="12"/>
       <c r="M18" s="13"/>
       <c r="N18" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="11">
         <v>6.25E-2</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="10">
-        <v>1.7361111111111112E-2</v>
-      </c>
-      <c r="E19" s="12">
-        <v>4.5138888888888888E-2</v>
-      </c>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E19" s="12"/>
       <c r="F19" s="10"/>
       <c r="G19" s="12"/>
       <c r="H19" s="10"/>
@@ -3697,21 +3819,23 @@
       <c r="L19" s="12"/>
       <c r="M19" s="13"/>
       <c r="N19" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="11">
-        <v>5.9027777777777783E-2</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="10"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="10">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="E20" s="12">
-        <v>5.9027777777777783E-2</v>
+        <v>4.5138888888888888E-2</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="12"/>
@@ -3722,18 +3846,22 @@
       <c r="L20" s="12"/>
       <c r="M20" s="13"/>
       <c r="N20" s="32">
-        <f t="shared" si="0"/>
-        <v>5.9027777777777783E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="11"/>
+        <v>25</v>
+      </c>
+      <c r="B21" s="11">
+        <v>5.9027777777777783E-2</v>
+      </c>
       <c r="C21" s="14"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="12"/>
+      <c r="E21" s="12">
+        <v>5.9027777777777783E-2</v>
+      </c>
       <c r="F21" s="10"/>
       <c r="G21" s="12"/>
       <c r="H21" s="10"/>
@@ -3743,13 +3871,13 @@
       <c r="L21" s="12"/>
       <c r="M21" s="13"/>
       <c r="N21" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5.9027777777777783E-2</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="14"/>
@@ -3764,43 +3892,39 @@
       <c r="L22" s="12"/>
       <c r="M22" s="13"/>
       <c r="N22" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>19</v>
+      <c r="A23" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="F23" s="10"/>
       <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
       <c r="L23" s="12"/>
       <c r="M23" s="13"/>
       <c r="N23" s="32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="11">
-        <v>6.25E-2</v>
-      </c>
+      <c r="A24" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="11"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
-      <c r="E24" s="12">
-        <v>6.25E-2</v>
-      </c>
+      <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
@@ -3810,27 +3934,25 @@
       <c r="L24" s="12"/>
       <c r="M24" s="13"/>
       <c r="N24" s="32">
-        <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="20">
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="C25" s="12">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D25" s="12">
-        <v>2.0833333333333332E-2</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B25" s="11">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="12">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="F25" s="12"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F25" s="12">
+        <v>5.9027777777777783E-2</v>
+      </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -3839,100 +3961,132 @@
       <c r="L25" s="12"/>
       <c r="M25" s="13"/>
       <c r="N25" s="32">
-        <f>SUM(C25:M25)</f>
-        <v>5.2083333333333329E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30" t="s">
+        <f t="shared" si="1"/>
+        <v>0.12152777777777779</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="20">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="C26" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D26" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E26" s="12">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F26" s="12">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="32">
+        <f>SUM(C26:M26)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B27" s="17">
         <v>0.17708333333333334</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C27" s="33">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D27" s="34">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E27" s="34">
         <v>0.11458333333333333</v>
       </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="32">
-        <f t="shared" si="0"/>
-        <v>0.17708333333333331</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="10">
-        <f>SUM(B2:B26)</f>
-        <v>1</v>
-      </c>
-      <c r="C27" s="10">
-        <f>SUM(C2:C26)</f>
+      <c r="F27" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="32">
+        <f t="shared" si="1"/>
+        <v>0.21874999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="10">
+        <f t="shared" ref="B28:M28" si="2">SUM(B2:B27)</f>
+        <v>0.97916666666666674</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" si="2"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="D27" s="10">
-        <f>SUM(D2:D26)</f>
+      <c r="D28" s="10">
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E27" s="10">
-        <f>SUM(E2:E26)</f>
+      <c r="E28" s="10">
+        <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F27" s="10">
-        <f>SUM(F2:F26)</f>
+      <c r="F28" s="10">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="G28" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G27" s="10">
-        <f>SUM(G2:G26)</f>
+      <c r="H28" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H27" s="10">
-        <f>SUM(H2:H26)</f>
+      <c r="I28" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I27" s="10">
-        <f>SUM(I2:I26)</f>
+      <c r="J28" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J27" s="10">
-        <f>SUM(J2:J26)</f>
+      <c r="K28" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K27" s="10">
-        <f>SUM(K2:K26)</f>
+      <c r="L28" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L27" s="10">
-        <f>SUM(L2:L26)</f>
+      <c r="M28" s="10">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M27" s="10">
-        <f>SUM(M2:M26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M28" s="10">
-        <f>SUM(C27:M27)</f>
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="N28" s="10">
-        <f>SUM(N2:N26)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="10">
+        <f>SUM(C28:M28)</f>
+        <v>1.333333333333333</v>
+      </c>
+      <c r="N29" s="10">
+        <f>SUM(N2:N27)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
     <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4904,224 +5058,295 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C6">
-    <cfRule type="cellIs" dxfId="48" priority="42" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="43" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="44" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5 I7:I22 G5 G7:G24 L5 L7:L24 C2:C26 E5:E26">
-    <cfRule type="cellIs" dxfId="45" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="59" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="60" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="61" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5 I7:I23 G5 G7:G25 L5 L7:L25 C2:C27 E5 E7:E27 E6:F6">
+    <cfRule type="cellIs" dxfId="59" priority="41" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="44" priority="25" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="28" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24:D25 F26:J26 L26:M26 F25:M25 F24:H24 D5 C7:D15 E7:M23 E2:M5">
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26:J26 C24:D25 F25:M25 F24:H24 C7:D15 E7:M23 D5:M5">
-    <cfRule type="cellIs" dxfId="40" priority="36" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26:J26 L26:M26 C24:D25 F25:M25 F24:H24 D5 C7:D15 E7:M23 E2:M5">
+  <conditionalFormatting sqref="C27">
+    <cfRule type="cellIs" dxfId="58" priority="42" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="44" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="45" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:D26 G27:J27 L27:M27 G26:M26 G25:H25 D5 C7:D16 E2:M2 G3:M5 G7:M24 F14:F24 E3:E24 F3:F12">
+    <cfRule type="cellIs" dxfId="55" priority="58" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27:J27 C25:D26 G26:M26 G25:H25 C7:D16 D5:E5 G5:M5 G7:M24 F14:F24 E6:E24 F6:F12">
+    <cfRule type="cellIs" dxfId="54" priority="53" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G27:J27 L27:M27 C25:D26 G26:M26 G25:H25 D5 C7:D16 E2:M2 G3:M5 G7:M24 F14:F24 E3:E24 F3:F12">
+    <cfRule type="cellIs" dxfId="53" priority="57" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:D25 G27:J27 L27:M27 G25:H25">
+    <cfRule type="cellIs" dxfId="52" priority="56" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:D24 C17:C20 D2:D4">
+    <cfRule type="cellIs" dxfId="51" priority="71" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:D24 G21:M24">
+    <cfRule type="cellIs" dxfId="50" priority="70" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:D24 D21:D23 C17:C23">
+    <cfRule type="cellIs" dxfId="49" priority="67" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:M28">
+    <cfRule type="cellIs" dxfId="48" priority="75" operator="equal">
+      <formula>0.333333333333333</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:D20">
+    <cfRule type="cellIs" dxfId="47" priority="32" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="34" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="35" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24 J24">
+    <cfRule type="cellIs" dxfId="44" priority="68" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25 H27 J27 M27">
+    <cfRule type="cellIs" dxfId="43" priority="54" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="42" priority="36" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="38" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="39" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="39" priority="40" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:D24 F26:J26 L26:M26 F24:H24">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20:D23 C16:C19 D2:D4">
-    <cfRule type="cellIs" dxfId="37" priority="54" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20:D23 F20:M23">
-    <cfRule type="cellIs" dxfId="36" priority="53" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23:D23 D20:D22 C16:C22">
-    <cfRule type="cellIs" dxfId="35" priority="50" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="34" priority="58" operator="equal">
-      <formula>0.333333333333333</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16:D19">
-    <cfRule type="cellIs" dxfId="33" priority="15" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="18" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23 J23">
-    <cfRule type="cellIs" dxfId="30" priority="51" operator="greaterThan">
+  <conditionalFormatting sqref="D27">
+    <cfRule type="cellIs" dxfId="38" priority="37" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24 F26 H26 J26 M26">
-    <cfRule type="cellIs" dxfId="29" priority="37" operator="greaterThan">
+  <conditionalFormatting sqref="D2:D4 C17:C20 C21:D24">
+    <cfRule type="cellIs" dxfId="37" priority="72" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D4 F2:M2 G3:M4">
+    <cfRule type="cellIs" dxfId="36" priority="63" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="28" priority="19" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="greaterThan">
+  <conditionalFormatting sqref="D2:D4 F2:M2 G3:M4">
+    <cfRule type="cellIs" dxfId="35" priority="64" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="cellIs" dxfId="34" priority="52" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4 C16:C19 C20:D23">
-    <cfRule type="cellIs" dxfId="23" priority="55" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4 F2:M4">
-    <cfRule type="cellIs" dxfId="22" priority="46" operator="greaterThan">
+  <conditionalFormatting sqref="G24">
+    <cfRule type="cellIs" dxfId="33" priority="69" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4 F2:M4">
-    <cfRule type="cellIs" dxfId="21" priority="47" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F23:F24 I26">
-    <cfRule type="cellIs" dxfId="20" priority="35" operator="greaterThan">
+  <conditionalFormatting sqref="G25:K25 K27:L27 D26 G27 G26:M26">
+    <cfRule type="cellIs" dxfId="32" priority="48" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G23">
-    <cfRule type="cellIs" dxfId="19" priority="52" operator="greaterThan">
+  <conditionalFormatting sqref="H24:I24">
+    <cfRule type="cellIs" dxfId="31" priority="66" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24:K24 K26:L26 D25 G26 F25:M25">
-    <cfRule type="cellIs" dxfId="18" priority="31" operator="greaterThan">
+  <conditionalFormatting sqref="I25:K25 K27">
+    <cfRule type="cellIs" dxfId="30" priority="47" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25:M25 K27">
+    <cfRule type="cellIs" dxfId="29" priority="50" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="51" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I25:M25 K27:M27">
+    <cfRule type="cellIs" dxfId="27" priority="49" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
+    <cfRule type="cellIs" dxfId="26" priority="65" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23:I23">
-    <cfRule type="cellIs" dxfId="17" priority="49" operator="greaterThan">
+  <conditionalFormatting sqref="M26">
+    <cfRule type="cellIs" dxfId="25" priority="46" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N27">
+    <cfRule type="cellIs" dxfId="24" priority="62" operator="equal">
+      <formula>$B2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E27">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E27">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27 E25:F25">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E27">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E13 E16:E24">
+    <cfRule type="cellIs" dxfId="19" priority="28" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24:K24 K26">
-    <cfRule type="cellIs" dxfId="16" priority="30" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24:M24 K26">
-    <cfRule type="cellIs" dxfId="15" priority="33" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="34" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24:M24 K26:M26">
-    <cfRule type="cellIs" dxfId="13" priority="32" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="12" priority="48" operator="greaterThan">
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:F6">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="20" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:F27">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:F27">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:F27">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16:F24">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M25">
-    <cfRule type="cellIs" dxfId="11" priority="29" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N26">
-    <cfRule type="cellIs" dxfId="10" priority="45" operator="equal">
-      <formula>$B2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24:E26">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24:E26">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24 E26">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24:E26">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E12 E15:E23">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E4">
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThan">
+  <conditionalFormatting sqref="F3:F5">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E4">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
+  <conditionalFormatting sqref="F3:F5">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mise à jour du TPI
fini l'affichage des jeux,  fin de la vue pour l'accueil
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijon Rahman\Documents\GitHub\Srijon_Rahman_TPI_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C28D19-069C-41BB-8375-C75997BAAA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDA72C0-1823-459D-AA87-E09E785AF8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,17 +489,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
-  <dxfs count="107">
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6D9F0"/>
-          <bgColor rgb="FFC6D9F0"/>
+  <dxfs count="115">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -528,6 +523,75 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6D9F0"/>
+          <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -547,14 +611,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB8CCE4"/>
-          <bgColor rgb="FFB8CCE4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1099,6 +1155,14 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFC6D9F0"/>
           <bgColor rgb="FFC6D9F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB8CCE4"/>
+          <bgColor rgb="FFB8CCE4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1571,7 +1635,7 @@
   <dimension ref="A1:AA999"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:F9"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3324,136 +3388,136 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="cellIs" dxfId="106" priority="16" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="17" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="16" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="17" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C25:J25 C24:M24">
-    <cfRule type="cellIs" dxfId="103" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C25:J25 L25:M25 C24:M24">
-    <cfRule type="cellIs" dxfId="102" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="101" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:H23 C24:M24 C25:J25 L25:M25">
-    <cfRule type="cellIs" dxfId="100" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="14" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:M22 D2:M4">
-    <cfRule type="cellIs" dxfId="99" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:M22">
-    <cfRule type="cellIs" dxfId="98" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="41" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:M22 C10:M11 D14:M21 C15:C21">
-    <cfRule type="cellIs" dxfId="97" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="36" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:M26">
-    <cfRule type="cellIs" dxfId="96" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="21" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22 J22">
-    <cfRule type="cellIs" dxfId="95" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="39" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23 D25 F25 H25 J25 M25">
-    <cfRule type="cellIs" dxfId="94" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="10" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M4 C5:M22">
-    <cfRule type="cellIs" dxfId="93" priority="43" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="43" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M4 I5:I21">
-    <cfRule type="cellIs" dxfId="92" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="27" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:M4">
-    <cfRule type="cellIs" dxfId="91" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:F23 I25">
-    <cfRule type="cellIs" dxfId="90" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="8" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G23">
-    <cfRule type="cellIs" dxfId="89" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="11" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="88" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="40" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23:K23 K25:L25 D24:M24 C2:C25 E5:E23 L5:L23 E25 G25">
-    <cfRule type="cellIs" dxfId="87" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="3" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:I22">
-    <cfRule type="cellIs" dxfId="86" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="35" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:K23 K25">
-    <cfRule type="cellIs" dxfId="85" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:M23 K25">
-    <cfRule type="cellIs" dxfId="84" priority="6" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:M23 K25:M25">
-    <cfRule type="cellIs" dxfId="82" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="81" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="89" priority="30" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M24">
-    <cfRule type="cellIs" dxfId="80" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N25">
-    <cfRule type="cellIs" dxfId="79" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="19" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3467,7 +3531,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3649,10 +3713,13 @@
       <c r="G6" s="25">
         <v>3.4722222222222224E-2</v>
       </c>
+      <c r="H6" s="25">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="M6" s="36"/>
       <c r="N6" s="32">
         <f t="shared" si="0"/>
-        <v>0.10069444444444445</v>
+        <v>0.12152777777777778</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3746,7 +3813,7 @@
       <c r="G10" s="25">
         <v>1.7361111111111112E-2</v>
       </c>
-      <c r="H10" s="25"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="21"/>
       <c r="J10" s="25"/>
       <c r="K10" s="25"/>
@@ -3769,7 +3836,6 @@
       <c r="G11" s="12">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="H11" s="10"/>
       <c r="I11" s="12"/>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -3791,7 +3857,9 @@
       <c r="G12" s="12">
         <v>2.4305555555555556E-2</v>
       </c>
-      <c r="H12" s="10"/>
+      <c r="H12" s="10">
+        <v>0.12847222222222224</v>
+      </c>
       <c r="I12" s="12"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -3799,7 +3867,7 @@
       <c r="M12" s="13"/>
       <c r="N12" s="32">
         <f t="shared" si="1"/>
-        <v>2.4305555555555556E-2</v>
+        <v>0.15277777777777779</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3812,7 +3880,6 @@
       <c r="E13" s="22"/>
       <c r="F13" s="25"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="25"/>
       <c r="I13" s="22"/>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
@@ -3839,7 +3906,6 @@
       <c r="E14" s="21"/>
       <c r="F14" s="25"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="25"/>
       <c r="I14" s="21"/>
       <c r="J14" s="25"/>
       <c r="K14" s="25"/>
@@ -3862,7 +3928,9 @@
       <c r="G15" s="15">
         <v>6.25E-2</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="10">
+        <v>3.8194444444444441E-2</v>
+      </c>
       <c r="I15" s="12"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
@@ -3870,7 +3938,7 @@
       <c r="M15" s="13"/>
       <c r="N15" s="32">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.10069444444444445</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4031,7 +4099,7 @@
       <c r="E22" s="12"/>
       <c r="F22" s="10"/>
       <c r="G22" s="12"/>
-      <c r="H22" s="10"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -4079,7 +4147,9 @@
         <v>5.9027777777777783E-2</v>
       </c>
       <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="H24" s="12">
+        <v>3.4722222222222224E-2</v>
+      </c>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
@@ -4087,7 +4157,7 @@
       <c r="M24" s="13"/>
       <c r="N24" s="32">
         <f t="shared" si="1"/>
-        <v>0.12152777777777779</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4112,7 +4182,9 @@
       <c r="G25" s="12">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="H25" s="12"/>
+      <c r="H25" s="12">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
@@ -4120,7 +4192,7 @@
       <c r="M25" s="13"/>
       <c r="N25" s="32">
         <f>SUM(C25:M25)</f>
-        <v>9.722222222222221E-2</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4145,7 +4217,9 @@
       <c r="G26" s="34">
         <v>3.8194444444444441E-2</v>
       </c>
-      <c r="H26" s="34"/>
+      <c r="H26" s="34">
+        <v>9.7222222222222224E-2</v>
+      </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
@@ -4153,7 +4227,7 @@
       <c r="M26" s="35"/>
       <c r="N26" s="32">
         <f t="shared" si="1"/>
-        <v>0.25694444444444442</v>
+        <v>0.35416666666666663</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4182,8 +4256,8 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="H27" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUM(H2:H26)</f>
+        <v>0.33333333333333337</v>
       </c>
       <c r="I27" s="10">
         <f t="shared" si="2"/>
@@ -4209,11 +4283,11 @@
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M28" s="10">
         <f>SUM(C27:M27)</f>
-        <v>1.6666666666666663</v>
+        <v>1.9999999999999996</v>
       </c>
       <c r="N28" s="10">
         <f>SUM(N2:N26)</f>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5190,359 +5264,414 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C6">
-    <cfRule type="cellIs" dxfId="78" priority="72" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="73" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="74" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5 L5 E5 E6:F6 G16:G24 I7:I22 L7:L24 C2:C26 E7:E26 G5:G10">
-    <cfRule type="cellIs" dxfId="6" priority="54" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="91" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="92" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="93" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5 L5 E5 E6:F6 G16:G24 I7:I22 L7:L24 C2:C26 E7:E26 G5:G10 H23 H25">
+    <cfRule type="cellIs" dxfId="83" priority="73" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="75" priority="55" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="57" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="58" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24:D25 H26:J26 L26:M26 H25:M25 G24:H24 D5 E2:M2 G3:M5 F13:F23 G16:M23 H11:M15 C7:D15 E3:E23 F3:F11 G7:M10">
-    <cfRule type="cellIs" dxfId="72" priority="71" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26:J26 C24:D25 H25:M25 G24:H24 D5:E5 G5:M5 F13:F23 G16:M23 H11:M15 C7:D15 E6:E23 F6:F11 G7:M10">
-    <cfRule type="cellIs" dxfId="71" priority="66" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26:J26 L26:M26 C24:D25 H25:M25 G24:H24 D5 E2:M2 G3:M5 F13:F23 G16:M23 H11:M15 C7:D15 E3:E23 F3:F11 G7:M10">
-    <cfRule type="cellIs" dxfId="70" priority="70" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24:D24 H26:J26 L26:M26 G24:H24">
-    <cfRule type="cellIs" dxfId="69" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="74" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="76" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="77" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:D25 H26:J26 L26:M26 I25:M25 D5 E2:G2 G3:G5 F13:F23 G16:G24 C7:D15 E3:E23 F3:F11 I7:M23 H25:H26 H2:M5 H15:H23 G7:H10 H12">
+    <cfRule type="cellIs" dxfId="79" priority="90" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26:J26 C24:D25 I25:M25 D5:E5 F13:F23 G16:G24 C7:D15 E6:E23 F6:F11 I7:M23 H25:H26 G5:M5 H15:H23 G7:H10 H12">
+    <cfRule type="cellIs" dxfId="78" priority="85" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26:J26 L26:M26 C24:D25 I25:M25 D5 E2:G2 G3:G5 F13:F23 G16:G24 C7:D15 E3:E23 F3:F11 I7:M23 H25:H26 H2:M5 H15:H23 G7:H10 H12">
+    <cfRule type="cellIs" dxfId="77" priority="89" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:D24 H26:J26 L26:M26 G24">
+    <cfRule type="cellIs" dxfId="76" priority="88" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:D23 C16:C19 D2:D4">
-    <cfRule type="cellIs" dxfId="68" priority="84" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20:D23 G20:M23">
-    <cfRule type="cellIs" dxfId="67" priority="83" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="103" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:D23 G20:G23 I20:M23">
+    <cfRule type="cellIs" dxfId="74" priority="102" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23:D23 D20:D22 C16:C22">
-    <cfRule type="cellIs" dxfId="66" priority="80" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="99" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:M27">
-    <cfRule type="cellIs" dxfId="65" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="107" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D19">
-    <cfRule type="cellIs" dxfId="64" priority="45" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="47" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="64" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="66" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="67" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23 J23">
-    <cfRule type="cellIs" dxfId="61" priority="81" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="100" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24 H26 J26 M26">
-    <cfRule type="cellIs" dxfId="60" priority="67" operator="greaterThan">
+  <conditionalFormatting sqref="D24 J26 M26">
+    <cfRule type="cellIs" dxfId="67" priority="86" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="59" priority="49" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="51" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="52" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="53" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="66" priority="68" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="70" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="71" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="72" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="55" priority="50" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="69" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D4 C16:C19 C20:D23">
-    <cfRule type="cellIs" dxfId="54" priority="85" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4 F2:M2 G3:M4">
-    <cfRule type="cellIs" dxfId="53" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="104" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D4 F2:G2 G3:G4 I2:M4">
+    <cfRule type="cellIs" dxfId="60" priority="95" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D4 F2:M2 G3:M4">
-    <cfRule type="cellIs" dxfId="52" priority="77" operator="greaterThan">
+  <conditionalFormatting sqref="D2:D4 F2:G2 G3:G4 I2:M4">
+    <cfRule type="cellIs" dxfId="59" priority="96" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26">
-    <cfRule type="cellIs" dxfId="51" priority="65" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="84" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G23">
-    <cfRule type="cellIs" dxfId="50" priority="82" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="101" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24:K24 K26:L26 D25 H25:M25">
-    <cfRule type="cellIs" dxfId="49" priority="61" operator="greaterThan">
+  <conditionalFormatting sqref="G24 K26:L26 D25 I25:M25 I24:K24">
+    <cfRule type="cellIs" dxfId="56" priority="80" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23:I23">
-    <cfRule type="cellIs" dxfId="48" priority="79" operator="greaterThan">
+  <conditionalFormatting sqref="I23">
+    <cfRule type="cellIs" dxfId="55" priority="98" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:K24 K26">
-    <cfRule type="cellIs" dxfId="47" priority="60" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="79" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:M24 K26">
-    <cfRule type="cellIs" dxfId="46" priority="63" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="82" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="83" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:M24 K26:M26">
-    <cfRule type="cellIs" dxfId="44" priority="62" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="81" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="43" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="97" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M25">
-    <cfRule type="cellIs" dxfId="42" priority="59" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="78" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N26">
-    <cfRule type="cellIs" dxfId="41" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="94" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:E26">
-    <cfRule type="cellIs" dxfId="40" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="54" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:E26">
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="56" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26 E24:F24">
-    <cfRule type="cellIs" dxfId="38" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="55" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:E26">
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="57" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:E12 E15:E23">
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="60" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="cellIs" dxfId="35" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="58" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="cellIs" dxfId="34" priority="40" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="59" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F6">
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="50" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="51" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="52" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:F26">
-    <cfRule type="cellIs" dxfId="30" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:F26">
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="cellIs" dxfId="28" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="41" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:F26">
-    <cfRule type="cellIs" dxfId="27" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:F23">
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="46" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="cellIs" dxfId="25" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="40" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F5">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="44" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F5">
-    <cfRule type="cellIs" dxfId="23" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="45" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="cellIs" dxfId="22" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="38" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="cellIs" dxfId="21" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="37" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="20" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="36" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="33" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="35" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G15">
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G15">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G12 G15">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G15">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="32" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11:G15">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="28" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25:G26">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25:G26">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="25" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25:G26">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="27" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25:G26">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="23" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
+  <conditionalFormatting sqref="G6:H6">
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:H6">
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6:H6">
+    <cfRule type="cellIs" dxfId="11" priority="21" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23 H26">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H4">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H4">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="cellIs" dxfId="6" priority="15" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>0.00001157407407</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
-      <formula>0</formula>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
TPI mis à jour
Factorisation du code, fin de la fonction pour la recherche, début de la page pour détaillé un jeu vidéo, ajout de quelque testes pour le plan le test.
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijon Rahman\Documents\GitHub\Srijon_Rahman_TPI_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDA72C0-1823-459D-AA87-E09E785AF8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD053564-C0DC-4789-99A2-F925FE8459CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,7 +155,7 @@
     <t>Insérer une base de données avec les différentes tables</t>
   </si>
   <si>
-    <t>CRUD de la table jeuvideo avec ses genres et ses plateformes et ses pegi</t>
+    <t>CRUD de la table jeuvideo avec ses genres et ses plateformes et ses contenu pegi</t>
   </si>
 </sst>
 </file>
@@ -3531,7 +3531,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3716,10 +3716,13 @@
       <c r="H6" s="25">
         <v>2.0833333333333332E-2</v>
       </c>
+      <c r="I6" s="25">
+        <v>2.4305555555555556E-2</v>
+      </c>
       <c r="M6" s="36"/>
       <c r="N6" s="32">
         <f t="shared" si="0"/>
-        <v>0.12152777777777778</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3860,14 +3863,16 @@
       <c r="H12" s="10">
         <v>0.12847222222222224</v>
       </c>
-      <c r="I12" s="12"/>
+      <c r="I12" s="12">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="12"/>
       <c r="M12" s="13"/>
       <c r="N12" s="32">
         <f t="shared" si="1"/>
-        <v>0.15277777777777779</v>
+        <v>0.16319444444444445</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4079,14 +4084,16 @@
       <c r="F21" s="10"/>
       <c r="G21" s="12"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="12"/>
+      <c r="I21" s="12">
+        <v>0.1423611111111111</v>
+      </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="12"/>
       <c r="M21" s="13"/>
       <c r="N21" s="32">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1423611111111111</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4136,7 +4143,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="11">
-        <v>6.25E-2</v>
+        <v>0.23611111111111113</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -4150,14 +4157,16 @@
       <c r="H24" s="12">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="I24" s="12"/>
+      <c r="I24" s="12">
+        <v>0.1076388888888889</v>
+      </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="13"/>
       <c r="N24" s="32">
         <f t="shared" si="1"/>
-        <v>0.15625</v>
+        <v>0.2638888888888889</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4165,7 +4174,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="20">
-        <v>5.2083333333333336E-2</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="C25" s="12">
         <v>2.0833333333333332E-2</v>
@@ -4185,14 +4194,16 @@
       <c r="H25" s="12">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="I25" s="12"/>
+      <c r="I25" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="13"/>
       <c r="N25" s="32">
         <f>SUM(C25:M25)</f>
-        <v>0.1111111111111111</v>
+        <v>0.13194444444444445</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4200,7 +4211,7 @@
         <v>33</v>
       </c>
       <c r="B26" s="17">
-        <v>0.17708333333333334</v>
+        <v>0.375</v>
       </c>
       <c r="C26" s="33">
         <v>2.0833333333333332E-2</v>
@@ -4220,20 +4231,22 @@
       <c r="H26" s="34">
         <v>9.7222222222222224E-2</v>
       </c>
-      <c r="I26" s="34"/>
+      <c r="I26" s="34">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
       <c r="L26" s="34"/>
       <c r="M26" s="35"/>
       <c r="N26" s="32">
         <f t="shared" si="1"/>
-        <v>0.35416666666666663</v>
+        <v>0.38194444444444442</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <f t="shared" ref="B27:M27" si="2">SUM(B2:B26)</f>
-        <v>0.97916666666666674</v>
+        <v>1.4305555555555556</v>
       </c>
       <c r="C27" s="10">
         <f t="shared" si="2"/>
@@ -4261,7 +4274,7 @@
       </c>
       <c r="I27" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J27" s="10">
         <f t="shared" si="2"/>
@@ -4283,11 +4296,11 @@
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M28" s="10">
         <f>SUM(C27:M27)</f>
-        <v>1.9999999999999996</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="N28" s="10">
         <f>SUM(N2:N26)</f>
-        <v>2</v>
+        <v>2.333333333333333</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5274,7 +5287,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5 L5 E5 E6:F6 G16:G24 I7:I22 L7:L24 C2:C26 E7:E26 G5:G10 H23 H25">
+  <conditionalFormatting sqref="I5 L5 E5 E6:F6 G16:G24 I7:I22 L7:L24 C2:C26 E7:E26 G5:G10 H23 H25:I25">
     <cfRule type="cellIs" dxfId="83" priority="73" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
@@ -5290,22 +5303,22 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:D25 H26:J26 L26:M26 I25:M25 D5 E2:G2 G3:G5 F13:F23 G16:G24 C7:D15 E3:E23 F3:F11 I7:M23 H25:H26 H2:M5 H15:H23 G7:H10 H12">
+  <conditionalFormatting sqref="C24:D25 L26:M26 D5 E2:G2 G3:G5 F13:F23 G16:G24 C7:D15 E3:E23 F3:F11 I7:M23 H25:H26 H2:M5 H15:H23 G7:H10 H12 H26:J26 I25:M25">
     <cfRule type="cellIs" dxfId="79" priority="90" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26:J26 C24:D25 I25:M25 D5:E5 F13:F23 G16:G24 C7:D15 E6:E23 F6:F11 I7:M23 H25:H26 G5:M5 H15:H23 G7:H10 H12">
+  <conditionalFormatting sqref="C24:D25 D5:E5 F13:F23 G16:G24 C7:D15 E6:E23 F6:F11 I7:M23 H25:H26 G5:M5 H15:H23 G7:H10 H12 H26:J26 I25:M25">
     <cfRule type="cellIs" dxfId="78" priority="85" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26:J26 L26:M26 C24:D25 I25:M25 D5 E2:G2 G3:G5 F13:F23 G16:G24 C7:D15 E3:E23 F3:F11 I7:M23 H25:H26 H2:M5 H15:H23 G7:H10 H12">
+  <conditionalFormatting sqref="L26:M26 C24:D25 D5 E2:G2 G3:G5 F13:F23 G16:G24 C7:D15 E3:E23 F3:F11 I7:M23 H25:H26 H2:M5 H15:H23 G7:H10 H12 H26:J26 I25:M25">
     <cfRule type="cellIs" dxfId="77" priority="89" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:D24 H26:J26 L26:M26 G24">
+  <conditionalFormatting sqref="C24:D24 L26:M26 G24 H26:J26">
     <cfRule type="cellIs" dxfId="76" priority="88" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -5395,7 +5408,7 @@
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24 K26:L26 D25 I25:M25 I24:K24">
+  <conditionalFormatting sqref="G24 K26:L26 D25 I25:M25 J24:K24">
     <cfRule type="cellIs" dxfId="56" priority="80" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
@@ -5405,12 +5418,12 @@
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24:K24 K26">
+  <conditionalFormatting sqref="J24:K24 K26">
     <cfRule type="cellIs" dxfId="54" priority="79" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24:M24 K26">
+  <conditionalFormatting sqref="J24:M24 K26">
     <cfRule type="cellIs" dxfId="53" priority="82" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -5418,7 +5431,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24:M24 K26:M26">
+  <conditionalFormatting sqref="J24:M24 K26:M26">
     <cfRule type="cellIs" dxfId="51" priority="81" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -5604,27 +5617,27 @@
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:H6">
+  <conditionalFormatting sqref="G6:I6">
     <cfRule type="cellIs" dxfId="13" priority="22" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:H6">
+  <conditionalFormatting sqref="G6:I6">
     <cfRule type="cellIs" dxfId="12" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:H6">
+  <conditionalFormatting sqref="G6:I6">
     <cfRule type="cellIs" dxfId="11" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23 H26">
+  <conditionalFormatting sqref="H23 H26:I26">
     <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26">
+  <conditionalFormatting sqref="H26:I26">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
@@ -5644,32 +5657,32 @@
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="H24:I24">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="H24:I24">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="H24:I24">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="H24:I24">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="H24:I24">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
+  <conditionalFormatting sqref="H6:I6">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mise à jour TPI 15.05.2023
Fin de la page d'édition de jeu vidéo, début du résumé TPI
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijon Rahman\Documents\GitHub\Srijon_Rahman_TPI_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FDA7A7-62E7-4671-B774-05F833628CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7B8A99-4BAF-4887-8919-375E0506F0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3537,7 +3537,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4119,12 +4119,14 @@
       <c r="J22" s="10">
         <v>7.9861111111111105E-2</v>
       </c>
-      <c r="K22" s="10"/>
+      <c r="K22" s="10">
+        <v>0.11458333333333333</v>
+      </c>
       <c r="L22" s="12"/>
       <c r="M22" s="13"/>
       <c r="N22" s="32">
         <f t="shared" si="1"/>
-        <v>7.9861111111111105E-2</v>
+        <v>0.19444444444444442</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4173,12 +4175,14 @@
       <c r="J24" s="12">
         <v>0.15625</v>
       </c>
-      <c r="K24" s="12"/>
+      <c r="K24" s="12">
+        <v>0.14583333333333334</v>
+      </c>
       <c r="L24" s="12"/>
       <c r="M24" s="13"/>
       <c r="N24" s="32">
         <f t="shared" si="1"/>
-        <v>0.4201388888888889</v>
+        <v>0.56597222222222221</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4212,12 +4216,14 @@
       <c r="J25" s="12">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="K25" s="12"/>
+      <c r="K25" s="12">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="L25" s="12"/>
       <c r="M25" s="13"/>
       <c r="N25" s="32">
         <f>SUM(C25:M25)</f>
-        <v>0.14583333333333334</v>
+        <v>0.1736111111111111</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4249,12 +4255,14 @@
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
+      <c r="K26" s="34">
+        <v>4.5138888888888888E-2</v>
+      </c>
       <c r="L26" s="34"/>
       <c r="M26" s="35"/>
       <c r="N26" s="32">
         <f t="shared" si="1"/>
-        <v>0.38194444444444442</v>
+        <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4296,7 +4304,7 @@
       </c>
       <c r="K27" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="L27" s="10">
         <f t="shared" si="2"/>
@@ -4310,11 +4318,11 @@
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M28" s="10">
         <f>SUM(C27:M27)</f>
-        <v>2.6666666666666665</v>
+        <v>3</v>
       </c>
       <c r="N28" s="10">
         <f>SUM(N2:N26)</f>
-        <v>2.666666666666667</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5422,7 +5430,7 @@
       <formula>0.00001157407407</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G24 K26:L26 D25 I25:M25 J24:K24">
+  <conditionalFormatting sqref="G24 K26:L26 D25 J24:K24 I25:M25">
     <cfRule type="cellIs" dxfId="56" priority="80" operator="greaterThan">
       <formula>0.00001157407407</formula>
     </cfRule>

</xml_diff>

<commit_message>
Mise à jour du TPI 16.05.2023
Bientôt la fin de toutes les tâches à faire pour le TPI. Début du manuel d'utilisateur.
</commit_message>
<xml_diff>
--- a/Planification.xlsx
+++ b/Planification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srijon Rahman\Documents\GitHub\Srijon_Rahman_TPI_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7B8A99-4BAF-4887-8919-375E0506F0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7D93FE-2880-4A32-BDB2-B066E076E623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3537,7 +3537,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3705,7 +3705,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="20">
-        <v>3.4722222222222224E-2</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="C6" s="21">
         <v>1.3888888888888888E-2</v>
@@ -3762,7 +3762,9 @@
       <c r="A8" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="20"/>
+      <c r="B8" s="20">
+        <v>0.20138888888888887</v>
+      </c>
       <c r="C8" s="21"/>
       <c r="D8" s="25"/>
       <c r="E8" s="21"/>
@@ -3787,7 +3789,9 @@
       <c r="A9" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="20">
+        <v>6.5972222222222224E-2</v>
+      </c>
       <c r="C9" s="21"/>
       <c r="D9" s="25"/>
       <c r="E9" s="21"/>
@@ -3812,7 +3816,9 @@
       <c r="A10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="20"/>
+      <c r="B10" s="20">
+        <v>7.6388888888888895E-2</v>
+      </c>
       <c r="C10" s="21"/>
       <c r="D10" s="25"/>
       <c r="E10" s="21"/>
@@ -3837,7 +3843,9 @@
       <c r="A11" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="11">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="C11" s="12"/>
       <c r="D11" s="10"/>
       <c r="E11" s="12"/>
@@ -3859,7 +3867,9 @@
       <c r="A12" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="11">
+        <v>0.16319444444444445</v>
+      </c>
       <c r="C12" s="12"/>
       <c r="D12" s="10"/>
       <c r="E12" s="12"/>
@@ -3931,7 +3941,9 @@
       <c r="A15" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="20"/>
+      <c r="B15" s="20">
+        <v>0.10069444444444443</v>
+      </c>
       <c r="C15" s="21"/>
       <c r="D15" s="10"/>
       <c r="E15" s="12"/>
@@ -4083,7 +4095,9 @@
       <c r="A21" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="11">
+        <v>0.22569444444444445</v>
+      </c>
       <c r="C21" s="14"/>
       <c r="D21" s="10"/>
       <c r="E21" s="12"/>
@@ -4108,7 +4122,9 @@
       <c r="A22" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="11"/>
+      <c r="B22" s="11">
+        <v>0.19444444444444445</v>
+      </c>
       <c r="C22" s="14"/>
       <c r="D22" s="10"/>
       <c r="E22" s="12"/>
@@ -4178,11 +4194,13 @@
       <c r="K24" s="12">
         <v>0.14583333333333334</v>
       </c>
-      <c r="L24" s="12"/>
+      <c r="L24" s="12">
+        <v>7.6388888888888895E-2</v>
+      </c>
       <c r="M24" s="13"/>
       <c r="N24" s="32">
         <f t="shared" si="1"/>
-        <v>0.56597222222222221</v>
+        <v>0.64236111111111116</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4219,11 +4237,13 @@
       <c r="K25" s="12">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="L25" s="12"/>
+      <c r="L25" s="12">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="M25" s="13"/>
       <c r="N25" s="32">
         <f>SUM(C25:M25)</f>
-        <v>0.1736111111111111</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4258,17 +4278,19 @@
       <c r="K26" s="34">
         <v>4.5138888888888888E-2</v>
       </c>
-      <c r="L26" s="34"/>
+      <c r="L26" s="34">
+        <v>0.24305555555555555</v>
+      </c>
       <c r="M26" s="35"/>
       <c r="N26" s="32">
         <f t="shared" si="1"/>
-        <v>0.42708333333333331</v>
+        <v>0.67013888888888884</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10">
         <f t="shared" ref="B27:M27" si="2">SUM(B2:B26)</f>
-        <v>1.4305555555555556</v>
+        <v>2.5763888888888888</v>
       </c>
       <c r="C27" s="10">
         <f t="shared" si="2"/>
@@ -4308,7 +4330,7 @@
       </c>
       <c r="L27" s="10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="M27" s="10">
         <f t="shared" si="2"/>
@@ -4318,11 +4340,11 @@
     <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M28" s="10">
         <f>SUM(C27:M27)</f>
-        <v>3</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="N28" s="10">
         <f>SUM(N2:N26)</f>
-        <v>3</v>
+        <v>3.3333333333333335</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>